<commit_message>
added text to execl file convertion code
</commit_message>
<xml_diff>
--- a/GEEPAS.xlsx
+++ b/GEEPAS.xlsx
@@ -34,10 +34,10 @@
     <t>https://geepasofficial.com</t>
   </si>
   <si>
+    <t>https://geepas.co.uk</t>
+  </si>
+  <si>
     <t>https://www.daraz.com.bd</t>
-  </si>
-  <si>
-    <t>https://geepas.co.uk</t>
   </si>
   <si>
     <t>https://www.shopz.com.bd</t>

</xml_diff>